<commit_message>
Created new mirth api service and updated some fields in model 1
</commit_message>
<xml_diff>
--- a/MirthConnect/Models_Features_HL7.xlsx
+++ b/MirthConnect/Models_Features_HL7.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaogu\OneDrive - Checkmarx\Documents\Tese\Mirth Connect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao Guedes\Desktop\Git Repos\ABI-Interoperability\MirthConnect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BAD1033-2ACD-45D2-A1B6-C9E0D7689B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A95C60A-0C08-45FA-A0C6-E0C3C6B0574C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-84" windowWidth="23256" windowHeight="12456" xr2:uid="{C70D916F-4E27-48A6-AB1A-5F19F9948B4D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C70D916F-4E27-48A6-AB1A-5F19F9948B4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,6 @@
     <t>HL7</t>
   </si>
   <si>
-    <t>ABI.2.1 (Custom Field)</t>
-  </si>
-  <si>
     <t>PVI.20.1 (Financial Class)</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>DG1.3.1 (Diagnosis Code)</t>
   </si>
   <si>
-    <t>OBX.5.1 (Observation Value)</t>
-  </si>
-  <si>
     <t>HORA_ADMISSAO</t>
   </si>
   <si>
@@ -117,13 +111,19 @@
   </si>
   <si>
     <t>custom</t>
+  </si>
+  <si>
+    <t>OBX.0.5.1 (Observation Value)</t>
+  </si>
+  <si>
+    <t>OBX.1.5.1 (Observation Value)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +133,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -160,9 +168,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -181,7 +190,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -477,19 +486,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB893B8-D76E-48DA-8DFA-23B891992F6E}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F9" sqref="F8:F9"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -497,128 +507,131 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
       <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>

</xml_diff>